<commit_message>
Deploying to gh-pages from  @ 19be8e76777f2131c28657fd85b4d8c07c6fc920 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.1.1.1a.xlsx
+++ b/en/downloads/data-excel/1.1.1.1a.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korozbaeva\Desktop\ПоказателиЦУР для Платформы\Национальные показатели ЦУР\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korozbaeva\Desktop\Показатели ЦУР для Платформы\Национальные показатели ЦУР\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -184,7 +184,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +266,33 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Times New Roman CE"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Times New Roman CE"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Times New Roman CE"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -342,7 +369,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -398,6 +425,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Normal 17" xfId="3"/>
@@ -8154,9 +8186,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
@@ -8165,7 +8199,7 @@
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="24" customHeight="1">
+    <row r="1" spans="1:14" ht="24" customHeight="1">
       <c r="A1" s="18" t="s">
         <v>22</v>
       </c>
@@ -8176,7 +8210,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.5" customHeight="1">
+    <row r="2" spans="1:14" ht="13.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -8187,7 +8221,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="12.75" thickBot="1">
+    <row r="3" spans="1:14" ht="12.75" thickBot="1">
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -8198,8 +8232,9 @@
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
+      <c r="N3" s="10"/>
     </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" thickBot="1">
+    <row r="4" spans="1:14" ht="15" customHeight="1" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -8239,8 +8274,11 @@
       <c r="M4" s="12">
         <v>2019</v>
       </c>
+      <c r="N4" s="19">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
@@ -8280,8 +8318,11 @@
       <c r="M5" s="14">
         <v>0.54933623931578479</v>
       </c>
+      <c r="N5" s="20">
+        <v>0.89148765717852163</v>
+      </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6" s="7" t="s">
         <v>24</v>
       </c>
@@ -8321,8 +8362,11 @@
       <c r="M6" s="15">
         <v>0.1</v>
       </c>
+      <c r="N6" s="21">
+        <v>0.31407178438278893</v>
+      </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14">
       <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
@@ -8362,8 +8406,11 @@
       <c r="M7" s="15">
         <v>0.8</v>
       </c>
+      <c r="N7" s="21">
+        <v>1.220561325080239</v>
+      </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8" s="9" t="s">
         <v>28</v>
       </c>
@@ -8403,8 +8450,11 @@
       <c r="M8" s="15">
         <v>0.3392671909690585</v>
       </c>
+      <c r="N8" s="22">
+        <v>1.6290305205827647</v>
+      </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="A9" s="9" t="s">
         <v>30</v>
       </c>
@@ -8444,8 +8494,11 @@
       <c r="M9" s="15">
         <v>0.56205045247263075</v>
       </c>
+      <c r="N9" s="22">
+        <v>1.4841131607226035</v>
+      </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14">
       <c r="A10" s="9" t="s">
         <v>32</v>
       </c>
@@ -8485,8 +8538,11 @@
       <c r="M10" s="15">
         <v>1.2604968981368243</v>
       </c>
+      <c r="N10" s="22">
+        <v>0.43494800834006392</v>
+      </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:14">
       <c r="A11" s="9" t="s">
         <v>34</v>
       </c>
@@ -8526,8 +8582,11 @@
       <c r="M11" s="15">
         <v>2.4816289901846873</v>
       </c>
+      <c r="N11" s="22">
+        <v>4.5037215639801795</v>
+      </c>
     </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1">
+    <row r="12" spans="1:14" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -8567,8 +8626,11 @@
       <c r="M12" s="15">
         <v>0.88079865305212723</v>
       </c>
+      <c r="N12" s="22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -8608,8 +8670,11 @@
       <c r="M13" s="15">
         <v>0</v>
       </c>
+      <c r="N13" s="22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -8649,8 +8714,11 @@
       <c r="M14" s="15">
         <v>0.16260204281171109</v>
       </c>
+      <c r="N14" s="22">
+        <v>1.3481169038547842</v>
+      </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
         <v>42</v>
       </c>
@@ -8690,8 +8758,11 @@
       <c r="M15" s="15">
         <v>0</v>
       </c>
+      <c r="N15" s="22">
+        <v>0.28229127286371936</v>
+      </c>
     </row>
-    <row r="16" spans="1:13" ht="12.75" thickBot="1">
+    <row r="16" spans="1:14" ht="12.75" thickBot="1">
       <c r="A16" s="10" t="s">
         <v>44</v>
       </c>
@@ -8729,6 +8800,9 @@
         <v>0.55610781362635098</v>
       </c>
       <c r="M16" s="17">
+        <v>0</v>
+      </c>
+      <c r="N16" s="23">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 726cf184c1908b9a3b1252f50b3618d7e2309dd2 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.1.1.1a.xlsx
+++ b/en/downloads/data-excel/1.1.1.1a.xlsx
@@ -39,12 +39,6 @@
     <t>Items</t>
   </si>
   <si>
-    <t>город</t>
-  </si>
-  <si>
-    <t>село</t>
-  </si>
-  <si>
     <t>1.1.1.1a Уровень крайней бедности</t>
   </si>
   <si>
@@ -81,12 +75,6 @@
     <t>Kyrgyz Republic</t>
   </si>
   <si>
-    <t>urban</t>
-  </si>
-  <si>
-    <t>rural</t>
-  </si>
-  <si>
     <t>…</t>
   </si>
   <si>
@@ -97,15 +85,6 @@
   </si>
   <si>
     <t>1.1.1.1а Деңгээли өтө жакырчылык калк</t>
-  </si>
-  <si>
-    <t>(жалпы санына каратапайыз менен)</t>
-  </si>
-  <si>
-    <t>шаар</t>
-  </si>
-  <si>
-    <t>айыл</t>
   </si>
   <si>
     <t>Кыргыз Республикасы</t>
@@ -175,6 +154,27 @@
   </si>
   <si>
     <t>*2013ж. чейин Ош ш. кошо алганда</t>
+  </si>
+  <si>
+    <t>Шаар жерлери</t>
+  </si>
+  <si>
+    <t>Городские поселения</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Айыл аймагы</t>
+  </si>
+  <si>
+    <t>Сельская местность</t>
+  </si>
+  <si>
+    <t>Village</t>
+  </si>
+  <si>
+    <t>(жалпы калктын санына карата пайыз менен)</t>
   </si>
 </sst>
 </file>
@@ -8188,8 +8188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -8201,24 +8201,24 @@
   <sheetData>
     <row r="1" spans="1:14" ht="24" customHeight="1">
       <c r="A1" s="18" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="13.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="12.75" thickBot="1">
@@ -8280,13 +8280,13 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="14">
         <v>5.3438169958924879</v>
@@ -8324,13 +8324,13 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="7" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="D6" s="15">
         <v>4.2168631530813512</v>
@@ -8368,13 +8368,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="8" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="D7" s="15">
         <v>5.9930922559799589</v>
@@ -8412,13 +8412,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="9" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D8" s="15">
         <v>5.1808804816231708</v>
@@ -8456,13 +8456,13 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="9" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D9" s="15">
         <v>6.4380322738993074</v>
@@ -8500,13 +8500,13 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D10" s="15">
         <v>2.4787267316625954</v>
@@ -8544,13 +8544,13 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D11" s="15">
         <v>12.036462028653192</v>
@@ -8588,13 +8588,13 @@
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D12" s="15">
         <v>8.3331494569001308</v>
@@ -8632,13 +8632,13 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D13" s="15">
         <v>5.0122940777216947</v>
@@ -8676,13 +8676,13 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D14" s="15">
         <v>3.5353129806100583</v>
@@ -8720,13 +8720,13 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D15" s="15">
         <v>0.53092532677015958</v>
@@ -8764,22 +8764,22 @@
     </row>
     <row r="16" spans="1:14" ht="12.75" thickBot="1">
       <c r="A16" s="10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G16" s="17">
         <v>3.5070632421313164</v>
@@ -8808,13 +8808,13 @@
     </row>
     <row r="17" spans="1:3" s="9" customFormat="1">
       <c r="A17" s="9" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 04b37270a010fe880d286a022aedc83c8ed46472 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.1.1.1a.xlsx
+++ b/en/downloads/data-excel/1.1.1.1a.xlsx
@@ -184,7 +184,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,6 +293,11 @@
       <family val="1"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Times New Roman CE"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -369,7 +374,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -430,6 +435,11 @@
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Normal 17" xfId="3"/>
@@ -8186,10 +8196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -8199,7 +8209,7 @@
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" customHeight="1">
+    <row r="1" spans="1:16" ht="24" customHeight="1">
       <c r="A1" s="18" t="s">
         <v>18</v>
       </c>
@@ -8210,7 +8220,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="13.5" customHeight="1">
+    <row r="2" spans="1:16" ht="13.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -8221,7 +8231,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="12.75" thickBot="1">
+    <row r="3" spans="1:16" ht="12.75" thickBot="1">
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -8233,8 +8243,10 @@
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
     </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" thickBot="1">
+    <row r="4" spans="1:16" ht="15" customHeight="1" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -8277,8 +8289,14 @@
       <c r="N4" s="19">
         <v>2020</v>
       </c>
+      <c r="O4" s="19">
+        <v>2021</v>
+      </c>
+      <c r="P4" s="28">
+        <v>2022</v>
+      </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:16">
       <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
@@ -8321,8 +8339,14 @@
       <c r="N5" s="20">
         <v>0.89148765717852163</v>
       </c>
+      <c r="O5" s="20">
+        <v>6.0337796775071091</v>
+      </c>
+      <c r="P5" s="24">
+        <v>5.9676405075953687</v>
+      </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:16">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -8365,8 +8389,14 @@
       <c r="N6" s="21">
         <v>0.31407178438278893</v>
       </c>
+      <c r="O6" s="25">
+        <v>7.3075058743442511</v>
+      </c>
+      <c r="P6" s="26">
+        <v>5.6044335798150424</v>
+      </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:16">
       <c r="A7" s="8" t="s">
         <v>45</v>
       </c>
@@ -8409,8 +8439,14 @@
       <c r="N7" s="21">
         <v>1.220561325080239</v>
       </c>
+      <c r="O7" s="25">
+        <v>5.2767607763499562</v>
+      </c>
+      <c r="P7" s="26">
+        <v>6.1789553077823856</v>
+      </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:16">
       <c r="A8" s="9" t="s">
         <v>21</v>
       </c>
@@ -8453,8 +8489,14 @@
       <c r="N8" s="22">
         <v>1.6290305205827647</v>
       </c>
+      <c r="O8" s="25">
+        <v>10.064200140319592</v>
+      </c>
+      <c r="P8" s="26">
+        <v>16.5</v>
+      </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:16">
       <c r="A9" s="9" t="s">
         <v>23</v>
       </c>
@@ -8497,8 +8539,14 @@
       <c r="N9" s="22">
         <v>1.4841131607226035</v>
       </c>
+      <c r="O9" s="25">
+        <v>7.5445007460298559</v>
+      </c>
+      <c r="P9" s="26">
+        <v>9.1</v>
+      </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:16">
       <c r="A10" s="9" t="s">
         <v>25</v>
       </c>
@@ -8541,8 +8589,14 @@
       <c r="N10" s="22">
         <v>0.43494800834006392</v>
       </c>
+      <c r="O10" s="25">
+        <v>7.9562092224762884</v>
+      </c>
+      <c r="P10" s="26">
+        <v>8.8000000000000007</v>
+      </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:16">
       <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
@@ -8585,8 +8639,14 @@
       <c r="N11" s="22">
         <v>4.5037215639801795</v>
       </c>
+      <c r="O11" s="25">
+        <v>8.1696953402867685</v>
+      </c>
+      <c r="P11" s="26">
+        <v>6.7</v>
+      </c>
     </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1">
+    <row r="12" spans="1:16" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -8629,8 +8689,14 @@
       <c r="N12" s="22">
         <v>0</v>
       </c>
+      <c r="O12" s="25">
+        <v>2.0701729813092102</v>
+      </c>
+      <c r="P12" s="26">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
         <v>31</v>
       </c>
@@ -8673,8 +8739,14 @@
       <c r="N13" s="22">
         <v>0</v>
       </c>
+      <c r="O13" s="25">
+        <v>2.6482523478927704</v>
+      </c>
+      <c r="P13" s="26">
+        <v>2.2000000000000002</v>
+      </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
@@ -8717,8 +8789,14 @@
       <c r="N14" s="22">
         <v>1.3481169038547842</v>
       </c>
+      <c r="O14" s="25">
+        <v>3.9561647100749857</v>
+      </c>
+      <c r="P14" s="26">
+        <v>5.0999999999999996</v>
+      </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
         <v>35</v>
       </c>
@@ -8761,8 +8839,14 @@
       <c r="N15" s="22">
         <v>0.28229127286371936</v>
       </c>
+      <c r="O15" s="25">
+        <v>9.4645167179465837</v>
+      </c>
+      <c r="P15" s="26">
+        <v>3.9</v>
+      </c>
     </row>
-    <row r="16" spans="1:14" ht="12.75" thickBot="1">
+    <row r="16" spans="1:16" ht="12.75" thickBot="1">
       <c r="A16" s="10" t="s">
         <v>37</v>
       </c>
@@ -8804,6 +8888,12 @@
       </c>
       <c r="N16" s="23">
         <v>0</v>
+      </c>
+      <c r="O16" s="27">
+        <v>3.1019579996103404</v>
+      </c>
+      <c r="P16" s="27">
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="9" customFormat="1">

</xml_diff>